<commit_message>
Backup de arquivos do mestrado (V1)
</commit_message>
<xml_diff>
--- a/Neural networks/teste de rede.xlsx
+++ b/Neural networks/teste de rede.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marci\Desktop\Projeto mestrado\Neural networks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E460507-057D-4A9E-9141-C0DE131C6623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3548F43C-B556-40DC-8836-39B60759DA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="108">
   <si>
     <t>Épocas</t>
   </si>
@@ -319,12 +319,6 @@
   </si>
   <si>
     <t>BATCH 06.04</t>
-  </si>
-  <si>
-    <t>A, B, Area_F</t>
-  </si>
-  <si>
-    <t>A, B, Vol_F</t>
   </si>
   <si>
     <t>A, B, Volume</t>
@@ -919,8 +913,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6441623" y="9470183"/>
-          <a:ext cx="2773134" cy="1369267"/>
+          <a:off x="6421509" y="9470183"/>
+          <a:ext cx="2775500" cy="1369267"/>
           <a:chOff x="5800727" y="6803183"/>
           <a:chExt cx="2762248" cy="1369267"/>
         </a:xfrm>
@@ -3400,23 +3394,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>305</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>319</xdr:row>
-      <xdr:rowOff>161533</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>612320</xdr:colOff>
+      <xdr:row>306</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>889019</xdr:colOff>
+      <xdr:row>324</xdr:row>
+      <xdr:rowOff>68035</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="41" name="Imagem 40">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA3763BB-945C-29BA-DF9B-253AA2507416}"/>
+        <xdr:cNvPr id="61" name="Imagem 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F11C387F-73A1-D75F-F239-2CD74BCA279B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3432,8 +3426,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8239125" y="58121550"/>
-          <a:ext cx="2905125" cy="2809483"/>
+          <a:off x="612320" y="58293000"/>
+          <a:ext cx="4562949" cy="3497035"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3444,23 +3438,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>305</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>523874</xdr:colOff>
-      <xdr:row>319</xdr:row>
-      <xdr:rowOff>143747</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>306</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>324</xdr:row>
+      <xdr:rowOff>156581</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="55" name="Imagem 54">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49E337B3-9682-69C5-1C85-F066EF0E8BE9}"/>
+        <xdr:cNvPr id="62" name="Imagem 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0D57904-F345-F5F3-3E69-856A4605E6BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3476,8 +3470,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11887200" y="58131075"/>
-          <a:ext cx="2952749" cy="2782172"/>
+          <a:off x="5810250" y="58293001"/>
+          <a:ext cx="3769179" cy="3585580"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3488,23 +3482,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>612320</xdr:colOff>
-      <xdr:row>306</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>330</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>889019</xdr:colOff>
-      <xdr:row>324</xdr:row>
-      <xdr:rowOff>68035</xdr:rowOff>
+      <xdr:colOff>884744</xdr:colOff>
+      <xdr:row>348</xdr:row>
+      <xdr:rowOff>122464</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="61" name="Imagem 60">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F11C387F-73A1-D75F-F239-2CD74BCA279B}"/>
+        <xdr:cNvPr id="63" name="Imagem 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{410B05A4-71D7-8BF9-61BF-747E71E7696B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3520,8 +3514,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="612320" y="58293000"/>
-          <a:ext cx="4562949" cy="3497035"/>
+          <a:off x="612322" y="62865001"/>
+          <a:ext cx="4558672" cy="3551463"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3534,21 +3528,21 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>306</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>324</xdr:row>
-      <xdr:rowOff>156581</xdr:rowOff>
+      <xdr:row>329</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>258536</xdr:colOff>
+      <xdr:row>348</xdr:row>
+      <xdr:rowOff>158314</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="62" name="Imagem 61">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0D57904-F345-F5F3-3E69-856A4605E6BD}"/>
+        <xdr:cNvPr id="64" name="Imagem 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF63FF08-ACDA-751D-2058-F6BF78A2C9D7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3564,8 +3558,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5810250" y="58293001"/>
-          <a:ext cx="3769179" cy="3585580"/>
+          <a:off x="5810250" y="62674500"/>
+          <a:ext cx="4544786" cy="3777814"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3577,22 +3571,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>330</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>353</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>884744</xdr:colOff>
-      <xdr:row>348</xdr:row>
-      <xdr:rowOff>122464</xdr:rowOff>
+      <xdr:colOff>905037</xdr:colOff>
+      <xdr:row>371</xdr:row>
+      <xdr:rowOff>27215</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="63" name="Imagem 62">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{410B05A4-71D7-8BF9-61BF-747E71E7696B}"/>
+        <xdr:cNvPr id="65" name="Imagem 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{097AA2D3-408E-8DD6-0E3E-2B90E387746C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3608,8 +3602,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="612322" y="62865001"/>
-          <a:ext cx="4558672" cy="3551463"/>
+          <a:off x="612321" y="67246501"/>
+          <a:ext cx="4578966" cy="3456214"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3622,21 +3616,21 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>329</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>258536</xdr:colOff>
-      <xdr:row>348</xdr:row>
-      <xdr:rowOff>158314</xdr:rowOff>
+      <xdr:row>352</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>340178</xdr:colOff>
+      <xdr:row>371</xdr:row>
+      <xdr:rowOff>176075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="64" name="Imagem 63">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF63FF08-ACDA-751D-2058-F6BF78A2C9D7}"/>
+        <xdr:cNvPr id="66" name="Imagem 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33110BE6-12E3-7C7D-1070-9C7264D34ACF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3652,8 +3646,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5810250" y="62674500"/>
-          <a:ext cx="4544786" cy="3777814"/>
+          <a:off x="5810250" y="67056001"/>
+          <a:ext cx="4014107" cy="3795574"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3666,21 +3660,21 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>353</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:row>377</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>905037</xdr:colOff>
-      <xdr:row>371</xdr:row>
-      <xdr:rowOff>27215</xdr:rowOff>
+      <xdr:colOff>867318</xdr:colOff>
+      <xdr:row>395</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="65" name="Imagem 64">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{097AA2D3-408E-8DD6-0E3E-2B90E387746C}"/>
+        <xdr:cNvPr id="67" name="Imagem 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F067340-CB9A-DF4F-CFBD-45A6FD7157BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3696,8 +3690,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="612321" y="67246501"/>
-          <a:ext cx="4578966" cy="3456214"/>
+          <a:off x="612321" y="71818500"/>
+          <a:ext cx="4541247" cy="3429000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3710,21 +3704,21 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>352</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:row>376</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>340178</xdr:colOff>
-      <xdr:row>371</xdr:row>
-      <xdr:rowOff>176075</xdr:rowOff>
+      <xdr:colOff>149678</xdr:colOff>
+      <xdr:row>394</xdr:row>
+      <xdr:rowOff>161063</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="66" name="Imagem 65">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33110BE6-12E3-7C7D-1070-9C7264D34ACF}"/>
+        <xdr:cNvPr id="68" name="Imagem 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5314E44E-4560-BFAD-6661-3FC614B8D959}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3740,8 +3734,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5810250" y="67056001"/>
-          <a:ext cx="4014107" cy="3795574"/>
+          <a:off x="5810250" y="71628000"/>
+          <a:ext cx="3823607" cy="3590063"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3753,22 +3747,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>377</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>867318</xdr:colOff>
-      <xdr:row>395</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>398</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>416</xdr:row>
+      <xdr:rowOff>30957</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="67" name="Imagem 66">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F067340-CB9A-DF4F-CFBD-45A6FD7157BA}"/>
+        <xdr:cNvPr id="69" name="Imagem 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD635D9E-6D8D-D3F6-593A-B926A0AC7724}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3784,8 +3778,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="612321" y="71818500"/>
-          <a:ext cx="4541247" cy="3429000"/>
+          <a:off x="612322" y="75819001"/>
+          <a:ext cx="4585608" cy="3459956"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3797,22 +3791,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>376</xdr:row>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>397</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>149678</xdr:colOff>
-      <xdr:row>394</xdr:row>
-      <xdr:rowOff>161063</xdr:rowOff>
+      <xdr:colOff>394608</xdr:colOff>
+      <xdr:row>416</xdr:row>
+      <xdr:rowOff>120379</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="68" name="Imagem 67">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5314E44E-4560-BFAD-6661-3FC614B8D959}"/>
+        <xdr:cNvPr id="70" name="Imagem 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{752E510F-289B-2221-2982-25CCB41FBD6C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3828,8 +3822,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5810250" y="71628000"/>
-          <a:ext cx="3823607" cy="3590063"/>
+          <a:off x="5810251" y="75628500"/>
+          <a:ext cx="4068536" cy="3739879"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3840,23 +3834,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>398</xdr:row>
+      <xdr:row>420</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>416</xdr:row>
-      <xdr:rowOff>30957</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>334914</xdr:colOff>
+      <xdr:row>439</xdr:row>
+      <xdr:rowOff>122465</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="69" name="Imagem 68">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD635D9E-6D8D-D3F6-593A-B926A0AC7724}"/>
+        <xdr:cNvPr id="71" name="Imagem 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82FD32ED-1183-8766-7EF9-0E4D8659C104}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3872,8 +3866,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="612322" y="75819001"/>
-          <a:ext cx="4585608" cy="3459956"/>
+          <a:off x="5810251" y="80010001"/>
+          <a:ext cx="4008842" cy="3741964"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3884,23 +3878,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>397</xdr:row>
+      <xdr:row>420</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>394608</xdr:colOff>
-      <xdr:row>416</xdr:row>
-      <xdr:rowOff>120379</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>891279</xdr:colOff>
+      <xdr:row>438</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="70" name="Imagem 69">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{752E510F-289B-2221-2982-25CCB41FBD6C}"/>
+        <xdr:cNvPr id="72" name="Imagem 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04C88BAF-C11C-017C-3012-E1527C810FED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3910,94 +3904,6 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5810251" y="75628500"/>
-          <a:ext cx="4068536" cy="3739879"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>420</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>334914</xdr:colOff>
-      <xdr:row>439</xdr:row>
-      <xdr:rowOff>122465</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="71" name="Imagem 70">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82FD32ED-1183-8766-7EF9-0E4D8659C104}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5810251" y="80010001"/>
-          <a:ext cx="4008842" cy="3741964"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>420</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>891279</xdr:colOff>
-      <xdr:row>438</xdr:row>
-      <xdr:rowOff>54429</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="72" name="Imagem 71">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04C88BAF-C11C-017C-3012-E1527C810FED}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4316,8 +4222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B7:AR450"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A309" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C304" sqref="C304"/>
+    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E146" sqref="E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4995,7 +4901,7 @@
         <v>97</v>
       </c>
       <c r="C303" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D303" s="3"/>
       <c r="E303" s="3"/>
@@ -5008,18 +4914,12 @@
       <c r="L303" s="3"/>
       <c r="M303" s="3"/>
     </row>
-    <row r="305" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
+        <v>98</v>
+      </c>
+      <c r="D305" t="s">
         <v>100</v>
-      </c>
-      <c r="D305" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG305" t="s">
-        <v>99</v>
-      </c>
-      <c r="AM305" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="323" spans="2:44" x14ac:dyDescent="0.25">
@@ -5027,15 +4927,15 @@
     </row>
     <row r="327" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="329" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D329" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="342" spans="2:24" x14ac:dyDescent="0.25">
@@ -5043,19 +4943,19 @@
     </row>
     <row r="352" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D352" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="374" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B374" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C374" s="3"/>
       <c r="D374" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E374" s="3"/>
       <c r="F374" s="3"/>
@@ -5069,26 +4969,26 @@
     </row>
     <row r="376" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D376" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="397" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B397" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F397" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="419" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F419" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="448" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>